<commit_message>
Report update current tets
</commit_message>
<xml_diff>
--- a/Report pieces/Current Noise.xlsx
+++ b/Report pieces/Current Noise.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="3">
   <si>
     <t>Mean</t>
   </si>
@@ -34,10 +34,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="#,##0.000"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
     <numFmt numFmtId="166" formatCode="0.00000"/>
+    <numFmt numFmtId="167" formatCode="0.0000"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -68,11 +69,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -353,10 +355,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:L7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="K1" sqref="K1:L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -365,7 +367,7 @@
     <col min="4" max="4" width="16.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -375,8 +377,20 @@
       <c r="D1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="H1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>-5.0956215908903797</v>
       </c>
@@ -387,29 +401,105 @@
         <f>STDEV(B2,B5)</f>
         <v>2.8336023966589541E-3</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="H2" s="2">
+        <v>-2.0049145985394701E-2</v>
+      </c>
+      <c r="I2" s="4">
+        <v>1.54883344613096E-3</v>
+      </c>
+      <c r="K2" s="2">
+        <v>-2.19183048009872E-2</v>
+      </c>
+      <c r="L2" s="4">
+        <v>1.4086166539250601E-3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>-5.0584883324550001</v>
       </c>
       <c r="B3" s="2">
         <v>5.4223559027976001E-2</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="H3" s="2">
+        <v>-0.55407472075987496</v>
+      </c>
+      <c r="I3" s="4">
+        <v>3.47865694172935E-3</v>
+      </c>
+      <c r="K3" s="2">
+        <v>0.68309141956960595</v>
+      </c>
+      <c r="L3" s="4">
+        <v>1.3433216525311001E-3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>-4.9150665993822003</v>
       </c>
       <c r="B4" s="2">
         <v>5.3890530445699997E-2</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="H4" s="2">
+        <v>-1.7582004540570799</v>
+      </c>
+      <c r="I4" s="4">
+        <v>1.1903179497765501E-2</v>
+      </c>
+      <c r="K4" s="2">
+        <v>1.56758007797856</v>
+      </c>
+      <c r="L4" s="4">
+        <v>1.5412683601421101E-3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>-5.0708577849082603</v>
       </c>
       <c r="B5" s="2">
         <v>5.6461729776168E-2</v>
+      </c>
+      <c r="H5" s="2">
+        <v>-2.7030293227134998</v>
+      </c>
+      <c r="I5" s="4">
+        <v>2.74058370014344E-2</v>
+      </c>
+      <c r="K5" s="2">
+        <v>2.3124645283159699</v>
+      </c>
+      <c r="L5" s="4">
+        <v>1.5530561628733499E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H6" s="2">
+        <v>-3.9636587916359201</v>
+      </c>
+      <c r="I6" s="4">
+        <v>3.5884466763871699E-2</v>
+      </c>
+      <c r="K6" s="2">
+        <v>3.18175477274134</v>
+      </c>
+      <c r="L6" s="4">
+        <v>1.56812179785935E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H7" s="2">
+        <v>-5.45401021605125</v>
+      </c>
+      <c r="I7" s="4">
+        <v>5.2305454467623198E-2</v>
+      </c>
+      <c r="K7" s="2">
+        <v>4.3161427320140797</v>
+      </c>
+      <c r="L7" s="4">
+        <v>2.23336432352688E-3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>